<commit_message>
fix(migration): deduplicate UES based on siren
</commit_message>
<xml_diff>
--- a/test/data/solen_ues.xlsx
+++ b/test/data/solen_ues.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="861">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="862">
   <si>
     <t xml:space="preserve">A répondu</t>
   </si>
@@ -2574,6 +2574,9 @@
   </si>
   <si>
     <t xml:space="preserve">UES500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BazBaz Three</t>
   </si>
   <si>
     <t xml:space="preserve">BazBaz One
@@ -2630,6 +2633,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2723,7 +2727,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -2733,7 +2737,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.1"/>
@@ -3886,17 +3890,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:TB2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S2" activeCellId="0" sqref="S2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.34"/>
   </cols>
@@ -5521,7 +5525,7 @@
         <v>309</v>
       </c>
       <c r="S2" s="0" t="s">
-        <v>310</v>
+        <v>851</v>
       </c>
       <c r="T2" s="0" t="n">
         <v>775701488</v>
@@ -5534,34 +5538,34 @@
       </c>
       <c r="W2" s="0"/>
       <c r="X2" s="4" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="Y2" s="4" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="Z2" s="4" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="AA2" s="4" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="AB2" s="4" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="AC2" s="4" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="AD2" s="4" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="AE2" s="4" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="AF2" s="4" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="AG2" s="4" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="AH2" s="0"/>
       <c r="AI2" s="0"/>
@@ -5598,7 +5602,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
chore(imports): validate solen imports before saving
</commit_message>
<xml_diff>
--- a/test/data/solen_ues.xlsx
+++ b/test/data/solen_ues.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="862">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="865">
   <si>
     <t xml:space="preserve">A répondu</t>
   </si>
@@ -935,7 +935,10 @@
     <t xml:space="preserve">Seine-Maritime</t>
   </si>
   <si>
-    <t xml:space="preserve">66 rue de FooBar 75000 BarBar</t>
+    <t xml:space="preserve">66 rue de FooBar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Barbar</t>
   </si>
   <si>
     <t xml:space="preserve">Unité Economique et Sociale (UES)</t>
@@ -2576,23 +2579,29 @@
     <t xml:space="preserve">UES500</t>
   </si>
   <si>
+    <t xml:space="preserve">66 rue de FooBar </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BarBar</t>
+  </si>
+  <si>
     <t xml:space="preserve">BazBaz Three</t>
   </si>
   <si>
     <t xml:space="preserve">BazBaz One
-423499322</t>
+423499326</t>
   </si>
   <si>
     <t xml:space="preserve">BazBaz Two
-344898355</t>
+344898358</t>
   </si>
   <si>
     <t xml:space="preserve">BazBaz Three
-775701488</t>
+775701485</t>
   </si>
   <si>
     <t xml:space="preserve">BazBaz Four
-500425666</t>
+500425665</t>
   </si>
   <si>
     <t xml:space="preserve">BazBaz Five
@@ -2600,15 +2609,15 @@
   </si>
   <si>
     <t xml:space="preserve">BazBaz Six
-434044000</t>
+434044004</t>
   </si>
   <si>
     <t xml:space="preserve">BazBaz Seven
-487597555</t>
+487597551</t>
   </si>
   <si>
     <t xml:space="preserve">BazBaz eight
-493147000</t>
+493147003</t>
   </si>
   <si>
     <t xml:space="preserve">BazBaz Nine
@@ -2616,7 +2625,7 @@
   </si>
   <si>
     <t xml:space="preserve">BazBaz Ten
-513866666</t>
+513866665</t>
   </si>
 </sst>
 </file>
@@ -2733,11 +2742,11 @@
   </sheetPr>
   <dimension ref="A1:KK2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Y2" activeCellId="0" sqref="Y2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.1"/>
@@ -3670,35 +3679,41 @@
       <c r="K2" s="0" t="s">
         <v>304</v>
       </c>
+      <c r="L2" s="1" t="n">
+        <v>76000</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>305</v>
+      </c>
       <c r="N2" s="1" t="n">
         <v>2018</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="S2" s="1" t="n">
         <v>6162</v>
       </c>
       <c r="W2" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="X2" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="Y2" s="0" t="n">
-        <v>775701488</v>
+        <v>775701485</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="AA2" s="1" t="n">
         <v>7</v>
@@ -3707,10 +3722,10 @@
         <v>43524</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="AD2" s="1" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="AE2" s="3" t="n">
         <v>43523</v>
@@ -3719,121 +3734,121 @@
         <v>7</v>
       </c>
       <c r="AZ2" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="BB2" s="1" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="BD2" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="BE2" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="BF2" s="1" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="BG2" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="BH2" s="1" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="BI2" s="1" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="BJ2" s="1" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="BK2" s="1" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="BL2" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="BM2" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="BN2" s="1" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="BO2" s="1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="BP2" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="BQ2" s="1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="BR2" s="1" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="BT2" s="1" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="BU2" s="1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="BV2" s="1" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="BX2" s="1" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="BY2" s="1" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="BZ2" s="1" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="IQ2" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="IR2" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="IS2" s="1" t="s">
         <v>297</v>
       </c>
       <c r="IV2" s="1" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="IW2" s="1" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="IX2" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="IY2" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="IZ2" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="JA2" s="1" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="JB2" s="1" t="s">
         <v>297</v>
       </c>
       <c r="JE2" s="1" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="JF2" s="1" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="JG2" s="1" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="JH2" s="1" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="JI2" s="1" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="JJ2" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="JK2" s="1" t="s">
         <v>297</v>
@@ -3845,7 +3860,7 @@
         <v>2</v>
       </c>
       <c r="JZ2" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="KA2" s="1" t="n">
         <v>38</v>
@@ -3854,10 +3869,10 @@
         <v>20</v>
       </c>
       <c r="KC2" s="1" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="KD2" s="1" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="KE2" s="1" t="n">
         <v>15</v>
@@ -3896,11 +3911,11 @@
   </sheetPr>
   <dimension ref="A1:TB2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S2" activeCellId="0" sqref="S2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AG2" activeCellId="0" sqref="AG2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.34"/>
   </cols>
@@ -3955,7 +3970,7 @@
         <v>15</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="R1" s="0" t="s">
         <v>22</v>
@@ -3973,1504 +3988,1504 @@
         <v>26</v>
       </c>
       <c r="W1" s="0" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="X1" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="Y1" s="0" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="Z1" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="AA1" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="AB1" s="0" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="AC1" s="0" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="AD1" s="0" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="AE1" s="0" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="AF1" s="0" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="AG1" s="0" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="AH1" s="0" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="AI1" s="0" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="AJ1" s="0" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="AK1" s="0" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="AL1" s="0" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="AM1" s="0" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="AN1" s="0" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="AO1" s="0" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="AP1" s="0" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="AQ1" s="0" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="AR1" s="0" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="AS1" s="0" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="AT1" s="0" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="AU1" s="0" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="AV1" s="0" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="AW1" s="0" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="AX1" s="0" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="AY1" s="0" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="AZ1" s="0" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="BA1" s="0" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="BB1" s="0" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="BC1" s="0" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="BD1" s="0" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="BE1" s="0" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="BF1" s="0" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="BG1" s="0" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="BH1" s="0" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="BI1" s="0" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="BJ1" s="0" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="BK1" s="0" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="BL1" s="0" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="BM1" s="1" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="BN1" s="1" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="BO1" s="1" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="BP1" s="1" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="BQ1" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="BR1" s="1" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="BS1" s="1" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="BT1" s="1" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="BU1" s="1" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="BV1" s="1" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="BW1" s="1" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="BX1" s="1" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="BY1" s="1" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="BZ1" s="1" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="CA1" s="1" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="CB1" s="1" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="CC1" s="1" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="CD1" s="1" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="CE1" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="CF1" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="CG1" s="1" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="CH1" s="1" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="CI1" s="1" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="CJ1" s="1" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="CK1" s="1" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="CL1" s="1" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="CM1" s="1" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="CN1" s="1" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="CO1" s="1" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="CP1" s="1" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="CQ1" s="1" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="CR1" s="1" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="CS1" s="1" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="CT1" s="1" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="CU1" s="1" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="CV1" s="1" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="CW1" s="1" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="CX1" s="1" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="CY1" s="1" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="CZ1" s="1" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="DA1" s="1" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="DB1" s="1" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="DC1" s="1" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="DD1" s="1" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="DE1" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="DF1" s="1" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="DG1" s="1" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="DH1" s="1" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="DI1" s="1" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="DJ1" s="1" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="DK1" s="1" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="DL1" s="1" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="DM1" s="1" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="DN1" s="1" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="DO1" s="1" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="DP1" s="1" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="DQ1" s="1" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="DR1" s="1" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="DS1" s="1" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="DT1" s="1" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="DU1" s="1" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="DV1" s="1" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="DW1" s="1" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="DX1" s="1" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="DY1" s="1" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="DZ1" s="1" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="EA1" s="1" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="EB1" s="1" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="EC1" s="1" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="ED1" s="1" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="EE1" s="1" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="EF1" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="EG1" s="1" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="EH1" s="1" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="EI1" s="1" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="EJ1" s="1" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="EK1" s="1" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="EL1" s="1" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="EM1" s="1" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="EN1" s="1" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="EO1" s="1" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="EP1" s="1" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="EQ1" s="1" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="ER1" s="1" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="ES1" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="ET1" s="1" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="EU1" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="EV1" s="1" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="EW1" s="1" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="EX1" s="1" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="EY1" s="1" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="EZ1" s="1" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="FA1" s="1" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="FB1" s="1" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="FC1" s="1" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="FD1" s="1" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="FE1" s="1" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="FF1" s="1" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="FG1" s="1" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="FH1" s="1" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="FI1" s="1" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="FJ1" s="1" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="FK1" s="1" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="FL1" s="1" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="FM1" s="1" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="FN1" s="1" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="FO1" s="1" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="FP1" s="1" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="FQ1" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="FR1" s="1" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="FS1" s="1" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="FT1" s="1" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="FU1" s="1" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="FV1" s="1" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="FW1" s="1" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="FX1" s="1" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="FY1" s="1" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="FZ1" s="1" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="GA1" s="1" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="GB1" s="1" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="GC1" s="1" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="GD1" s="1" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="GE1" s="1" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="GF1" s="1" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="GG1" s="1" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="GH1" s="1" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="GI1" s="1" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="GJ1" s="1" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="GK1" s="1" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="GL1" s="1" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="GM1" s="1" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="GN1" s="1" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="GO1" s="1" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="GP1" s="1" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="GQ1" s="1" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="GR1" s="1" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="GS1" s="1" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="GT1" s="1" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="GU1" s="1" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="GV1" s="1" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="GW1" s="1" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="GX1" s="1" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="GY1" s="1" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="GZ1" s="1" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="HA1" s="1" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="HB1" s="1" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="HC1" s="1" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="HD1" s="1" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="HE1" s="1" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="HF1" s="1" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="HG1" s="1" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="HH1" s="1" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="HI1" s="1" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="HJ1" s="1" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="HK1" s="1" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="HL1" s="1" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="HM1" s="1" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="HN1" s="1" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="HO1" s="1" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="HP1" s="1" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="HQ1" s="1" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="HR1" s="1" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="HS1" s="1" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="HT1" s="1" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="HU1" s="1" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="HV1" s="1" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="HW1" s="1" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="HX1" s="1" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="HY1" s="1" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="HZ1" s="1" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="IA1" s="1" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="IB1" s="1" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="IC1" s="1" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="ID1" s="1" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="IE1" s="1" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="IF1" s="1" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="IG1" s="1" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="IH1" s="1" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="II1" s="1" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="IJ1" s="1" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="IK1" s="1" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="IL1" s="1" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="IM1" s="1" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="IN1" s="1" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="IO1" s="1" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="IP1" s="1" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="IQ1" s="1" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="IR1" s="1" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="IS1" s="1" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="IT1" s="1" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="IU1" s="1" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="IV1" s="1" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="IW1" s="1" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="IX1" s="1" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="IY1" s="1" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="IZ1" s="1" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="JA1" s="1" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="JB1" s="1" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="JC1" s="1" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="JD1" s="1" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="JE1" s="1" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="JF1" s="1" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="JG1" s="1" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="JH1" s="1" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="JI1" s="1" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="JJ1" s="1" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="JK1" s="1" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="JL1" s="1" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="JM1" s="1" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="JN1" s="1" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="JO1" s="1" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="JP1" s="1" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="JQ1" s="1" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="JR1" s="1" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="JS1" s="1" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="JT1" s="1" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="JU1" s="1" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="JV1" s="1" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="JW1" s="1" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="JX1" s="1" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="JY1" s="1" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="JZ1" s="1" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="KA1" s="1" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="KB1" s="1" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="KC1" s="1" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="KD1" s="1" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="KE1" s="1" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="KF1" s="1" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="KG1" s="1" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="KH1" s="1" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="KI1" s="1" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="KJ1" s="1" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="KK1" s="1" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="KL1" s="1" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="KM1" s="1" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="KN1" s="1" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="KO1" s="1" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="KP1" s="1" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="KQ1" s="1" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="KR1" s="1" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="KS1" s="1" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="KT1" s="1" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="KU1" s="1" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="KV1" s="1" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="KW1" s="1" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="KX1" s="1" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="KY1" s="1" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="KZ1" s="1" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="LA1" s="1" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="LB1" s="1" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="LC1" s="1" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="LD1" s="1" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="LE1" s="1" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="LF1" s="1" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="LG1" s="1" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="LH1" s="1" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="LI1" s="1" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="LJ1" s="1" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="LK1" s="1" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="LL1" s="1" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="LM1" s="1" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="LN1" s="1" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="LO1" s="1" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="LP1" s="1" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="LQ1" s="1" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="LR1" s="1" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="LS1" s="1" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="LT1" s="1" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="LU1" s="1" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="LV1" s="1" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="LW1" s="1" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="LX1" s="1" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="LY1" s="1" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="LZ1" s="1" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="MA1" s="1" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="MB1" s="1" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="MC1" s="1" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="MD1" s="1" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="ME1" s="1" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="MF1" s="1" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="MG1" s="1" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="MH1" s="1" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="MI1" s="1" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="MJ1" s="1" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="MK1" s="1" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="ML1" s="1" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="MM1" s="1" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="MN1" s="1" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="MO1" s="1" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="MP1" s="1" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="MQ1" s="1" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="MR1" s="1" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="MS1" s="1" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="MT1" s="1" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="MU1" s="1" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="MV1" s="1" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="MW1" s="1" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="MX1" s="1" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="MY1" s="1" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="MZ1" s="1" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="NA1" s="1" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="NB1" s="1" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="NC1" s="1" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="ND1" s="1" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="NE1" s="1" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="NF1" s="1" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="NG1" s="1" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="NH1" s="1" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="NI1" s="1" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="NJ1" s="1" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="NK1" s="1" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="NL1" s="1" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="NM1" s="1" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="NN1" s="1" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="NO1" s="1" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="NP1" s="1" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="NQ1" s="1" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="NR1" s="1" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="NS1" s="1" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="NT1" s="1" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="NU1" s="1" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="NV1" s="1" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="NW1" s="1" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="NX1" s="1" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="NY1" s="1" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="NZ1" s="1" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="OA1" s="1" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="OB1" s="1" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="OC1" s="1" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="OD1" s="1" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="OE1" s="1" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="OF1" s="1" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="OG1" s="1" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="OH1" s="1" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="OI1" s="1" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="OJ1" s="1" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="OK1" s="1" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="OL1" s="1" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="OM1" s="1" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="ON1" s="1" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="OO1" s="1" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="OP1" s="1" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="OQ1" s="1" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="OR1" s="1" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="OS1" s="1" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="OT1" s="1" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="OU1" s="1" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="OV1" s="1" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="OW1" s="1" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="OX1" s="1" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="OY1" s="1" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="OZ1" s="1" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="PA1" s="1" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="PB1" s="1" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="PC1" s="1" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="PD1" s="1" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="PE1" s="1" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="PF1" s="1" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="PG1" s="1" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="PH1" s="1" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="PI1" s="1" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="PJ1" s="1" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="PK1" s="1" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="PL1" s="1" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="PM1" s="1" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="PN1" s="1" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="PO1" s="1" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="PP1" s="1" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="PQ1" s="1" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="PR1" s="1" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="PS1" s="1" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="PT1" s="1" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="PU1" s="1" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="PV1" s="1" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="PW1" s="1" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="PX1" s="1" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="PY1" s="1" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="PZ1" s="1" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="QA1" s="1" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="QB1" s="1" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="QC1" s="1" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="QD1" s="1" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="QE1" s="1" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="QF1" s="1" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="QG1" s="1" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="QH1" s="1" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="QI1" s="1" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="QJ1" s="1" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="QK1" s="1" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="QL1" s="1" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="QM1" s="1" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="QN1" s="1" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="QO1" s="1" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="QP1" s="1" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="QQ1" s="1" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="QR1" s="1" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="QS1" s="1" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="QT1" s="1" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="QU1" s="1" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="QV1" s="1" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="QW1" s="1" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="QX1" s="1" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="QY1" s="1" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="QZ1" s="1" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="RA1" s="1" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="RB1" s="1" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="RC1" s="1" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="RD1" s="1" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="RE1" s="1" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="RF1" s="1" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="RG1" s="1" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="RH1" s="1" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="RI1" s="1" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="RJ1" s="1" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="RK1" s="1" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="RL1" s="1" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="RM1" s="1" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="RN1" s="1" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="RO1" s="1" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="RP1" s="1" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="RQ1" s="1" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="RR1" s="1" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="RS1" s="1" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="RT1" s="1" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="RU1" s="1" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="RV1" s="1" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="RW1" s="1" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="RX1" s="1" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="RY1" s="1" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="RZ1" s="1" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="SA1" s="1" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="SB1" s="1" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="SC1" s="1" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="SD1" s="1" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="SE1" s="1" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="SF1" s="1" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="SG1" s="1" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="SH1" s="1" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="SI1" s="1" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="SJ1" s="1" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="SK1" s="1" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="SL1" s="1" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="SM1" s="1" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="SN1" s="1" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="SO1" s="1" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="SP1" s="1" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="SQ1" s="1" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="SR1" s="1" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="SS1" s="1" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="ST1" s="1" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="SU1" s="1" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="SV1" s="1" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="SW1" s="1" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="SX1" s="1" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="SY1" s="1" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="SZ1" s="1" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="TA1" s="1" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="TB1" s="1" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="true" ht="34.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5505,67 +5520,71 @@
         <v>303</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>304</v>
-      </c>
-      <c r="L2" s="0"/>
-      <c r="M2" s="0"/>
+        <v>852</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>75000</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>853</v>
+      </c>
       <c r="N2" s="0" t="n">
         <v>2018</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="Q2" s="0" t="n">
         <v>6162</v>
       </c>
       <c r="R2" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="S2" s="0" t="s">
-        <v>851</v>
+        <v>854</v>
       </c>
       <c r="T2" s="0" t="n">
         <v>775701488</v>
       </c>
       <c r="U2" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="V2" s="0" t="n">
         <v>7</v>
       </c>
       <c r="W2" s="0"/>
       <c r="X2" s="4" t="s">
-        <v>852</v>
+        <v>855</v>
       </c>
       <c r="Y2" s="4" t="s">
-        <v>853</v>
+        <v>856</v>
       </c>
       <c r="Z2" s="4" t="s">
-        <v>854</v>
+        <v>857</v>
       </c>
       <c r="AA2" s="4" t="s">
-        <v>855</v>
+        <v>858</v>
       </c>
       <c r="AB2" s="4" t="s">
-        <v>856</v>
+        <v>859</v>
       </c>
       <c r="AC2" s="4" t="s">
-        <v>857</v>
+        <v>860</v>
       </c>
       <c r="AD2" s="4" t="s">
-        <v>858</v>
+        <v>861</v>
       </c>
       <c r="AE2" s="4" t="s">
-        <v>859</v>
+        <v>862</v>
       </c>
       <c r="AF2" s="4" t="s">
-        <v>860</v>
+        <v>863</v>
       </c>
       <c r="AG2" s="4" t="s">
-        <v>861</v>
+        <v>864</v>
       </c>
       <c r="AH2" s="0"/>
       <c r="AI2" s="0"/>

</xml_diff>